<commit_message>
added few more components
</commit_message>
<xml_diff>
--- a/Sample Files/Test.xlsx
+++ b/Sample Files/Test.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23298F35-FBA5-4470-AD4B-3B00351E34DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E111799-7CF4-4D1C-87C5-69A6847DB1E0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +30,24 @@
   </si>
   <si>
     <t>Desmond</t>
+  </si>
+  <si>
+    <t>Rich</t>
+  </si>
+  <si>
+    <t>Bae</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Merge</t>
   </si>
 </sst>
 </file>
@@ -52,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -60,12 +79,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -375,4 +440,111 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BE5C46-949E-43E5-9826-540102F6F075}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>